<commit_message>
Updated BOM to reflect purchased components
</commit_message>
<xml_diff>
--- a/PCB/DE10-lite_shield/DE10-lite_shield_bom.xlsx
+++ b/PCB/DE10-lite_shield/DE10-lite_shield_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Uni\Year_2\Design_Project_2\EEEBalanceBug\PCB\DE10-lite_shield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E11F5CB-8247-4A94-B73D-89339B409323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539A7E75-ED03-4A57-8E3E-3632FCBE1CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{B4AE7691-1ECF-41CD-A3D4-186728AF4D5B}"/>
+    <workbookView xWindow="13560" yWindow="3840" windowWidth="21585" windowHeight="15240" xr2:uid="{B4AE7691-1ECF-41CD-A3D4-186728AF4D5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>CP2102N-A02-GQFN28</t>
   </si>
@@ -580,15 +580,15 @@
   <dimension ref="B2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -608,7 +608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -631,19 +631,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>7</v>
+      </c>
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -666,7 +671,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -689,7 +694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -712,7 +717,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -735,7 +740,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>29</v>
       </c>
@@ -758,7 +763,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>31</v>
       </c>
@@ -781,7 +786,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>36</v>
       </c>
@@ -804,7 +809,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>31.8201</v>
       </c>
@@ -827,7 +832,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>42</v>
       </c>
@@ -847,7 +852,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>44</v>
       </c>
@@ -860,11 +865,14 @@
       <c r="E14">
         <v>100</v>
       </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
       <c r="H14" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>46</v>
       </c>
@@ -877,14 +885,17 @@
       <c r="E15">
         <v>10</v>
       </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
       <c r="H15" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" s="2" cm="1">
         <f t="array" ref="E17">SUM(D3:D16*E3:E16)</f>
-        <v>17.898</v>
+        <v>24.898</v>
       </c>
       <c r="F17" s="2"/>
     </row>

</xml_diff>